<commit_message>
Reajustando o visual da cotação
</commit_message>
<xml_diff>
--- a/planos_de_saude_unificado.xlsx
+++ b/planos_de_saude_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Torres\Documents\IDPB\cotacao-plano-saude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDF75BD-EBCC-4901-AC4C-659A06A39DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6E7C1E-CF99-4E7D-BA52-197E5D0D7AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>Empresa</t>
   </si>
   <si>
-    <t>Tipo Plano</t>
-  </si>
-  <si>
     <t>Idade</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Tipo de Plano</t>
   </si>
 </sst>
 </file>
@@ -172,7 +172,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -482,7 +482,7 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,6 +492,7 @@
     <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -499,30 +500,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>305.06</v>
@@ -531,18 +532,18 @@
         <v>455.72</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>401.49</v>
@@ -551,18 +552,18 @@
         <v>600.36</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>461.16</v>
@@ -571,18 +572,18 @@
         <v>689.36</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>516.04999999999995</v>
@@ -591,18 +592,18 @@
         <v>772.2</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>541.66999999999996</v>
@@ -611,18 +612,18 @@
         <v>810.62</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>611.6</v>
@@ -631,18 +632,18 @@
         <v>915.52</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>745.34</v>
@@ -651,18 +652,18 @@
         <v>1116.1199999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>1027.1600000000001</v>
@@ -671,18 +672,18 @@
         <v>1538.46</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>1385.37</v>
@@ -691,18 +692,18 @@
         <v>2076.14</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>1799.87</v>
@@ -711,18 +712,18 @@
         <v>2697.87</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>218.02</v>
@@ -731,18 +732,18 @@
         <v>325.16000000000003</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>286.60000000000002</v>
@@ -751,18 +752,18 @@
         <v>428.02</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>329.03</v>
@@ -771,18 +772,18 @@
         <v>491.67</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>368.07</v>
@@ -791,18 +792,18 @@
         <v>550.23</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>386.29</v>
@@ -811,18 +812,18 @@
         <v>577.55999999999995</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17">
         <v>436.03</v>
@@ -831,18 +832,18 @@
         <v>652.16</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>531.14</v>
@@ -851,18 +852,18 @@
         <v>794.82</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>731.56</v>
@@ -871,18 +872,18 @@
         <v>1095.44</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20">
         <v>986.31</v>
@@ -891,18 +892,18 @@
         <v>1477.55</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21">
         <v>1281.0899999999999</v>
@@ -911,18 +912,18 @@
         <v>1919.7</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>281.39</v>
@@ -931,18 +932,18 @@
         <v>393.95</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <v>371.43</v>
@@ -951,18 +952,18 @@
         <v>520.01</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24">
         <v>427.15</v>
@@ -971,18 +972,18 @@
         <v>598.01</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>478.41</v>
@@ -991,18 +992,18 @@
         <v>669.77</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <v>526.25</v>
@@ -1011,18 +1012,18 @@
         <v>736.75</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27">
         <v>594.66</v>
@@ -1031,18 +1032,18 @@
         <v>832.53</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>725.49</v>
@@ -1051,18 +1052,18 @@
         <v>1015.68</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29">
         <v>1008.43</v>
@@ -1071,18 +1072,18 @@
         <v>1411.8</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30">
         <v>1371.46</v>
@@ -1091,18 +1092,18 @@
         <v>1920.04</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D31">
         <v>1686.9</v>
@@ -1111,18 +1112,18 @@
         <v>2361.65</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <v>215.92</v>
@@ -1131,18 +1132,18 @@
         <v>302.29000000000002</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33">
         <v>285.02</v>
@@ -1151,18 +1152,18 @@
         <v>399.03</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>327.77</v>
@@ -1171,18 +1172,18 @@
         <v>458.88</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <v>367.1</v>
@@ -1191,18 +1192,18 @@
         <v>513.94000000000005</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36">
         <v>403.81</v>
@@ -1211,18 +1212,18 @@
         <v>565.34</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37">
         <v>456.38</v>
@@ -1231,18 +1232,18 @@
         <v>638.84</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D38">
         <v>556.70000000000005</v>
@@ -1251,18 +1252,18 @@
         <v>779.37</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D39">
         <v>773.81</v>
@@ -1271,18 +1272,18 @@
         <v>1083.33</v>
       </c>
       <c r="F39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <v>1052.3900000000001</v>
@@ -1291,18 +1292,18 @@
         <v>1473.34</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D41">
         <v>1294.43</v>
@@ -1311,607 +1312,607 @@
         <v>1812.2</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
         <v>7</v>
-      </c>
-      <c r="B42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
       </c>
       <c r="D42">
         <v>373.13</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43">
         <v>442.9</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <v>531.48</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D45">
         <v>593.67999999999995</v>
       </c>
       <c r="E45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>664.91</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47">
         <v>819.96</v>
       </c>
       <c r="E47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48">
         <v>914.02</v>
       </c>
       <c r="E48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49">
         <v>1269.1199999999999</v>
       </c>
       <c r="E49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D50">
         <v>1785.8</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D51">
         <v>2234.34</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" t="s">
         <v>7</v>
-      </c>
-      <c r="B52" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
       </c>
       <c r="D52">
         <v>594.27</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D53">
         <v>760.63</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D54">
         <v>808.05</v>
       </c>
       <c r="E54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D55">
         <v>831.82</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56">
         <v>909.05</v>
       </c>
       <c r="E56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D57">
         <v>1039.76</v>
       </c>
       <c r="E57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D58">
         <v>1455.73</v>
       </c>
       <c r="E58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59">
         <v>1948.96</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D60">
         <v>2186.75</v>
       </c>
       <c r="E60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D61">
         <v>3565.09</v>
       </c>
       <c r="E61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
         <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" t="s">
-        <v>8</v>
       </c>
       <c r="D62">
         <v>295.92</v>
       </c>
       <c r="E62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D63">
         <v>378.77</v>
       </c>
       <c r="E63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D64">
         <v>402.44</v>
       </c>
       <c r="E64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D65">
         <v>414.23</v>
       </c>
       <c r="E65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D66">
         <v>452.7</v>
       </c>
       <c r="E66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D67">
         <v>517.79999999999995</v>
       </c>
       <c r="E67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F67" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D68">
         <v>724.9</v>
       </c>
       <c r="E68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D69">
         <v>970.51</v>
       </c>
       <c r="E69" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D70">
         <v>1088.9000000000001</v>
       </c>
       <c r="E70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F70" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D71">
         <v>1775.35</v>
       </c>
       <c r="E71" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F71" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado login e lógica de validade do plano
</commit_message>
<xml_diff>
--- a/planos_de_saude_unificado.xlsx
+++ b/planos_de_saude_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Torres\Documents\IDPB\cotacao-plano-saude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6E7C1E-CF99-4E7D-BA52-197E5D0D7AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76031E29-1C3D-44C9-86EE-C817E1380E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="29">
   <si>
     <t>Empresa</t>
   </si>
@@ -98,13 +98,22 @@
   </si>
   <si>
     <t>Tipo de Plano</t>
+  </si>
+  <si>
+    <t>Validade</t>
+  </si>
+  <si>
+    <t>2025-12</t>
+  </si>
+  <si>
+    <t>2025-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +125,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,12 +182,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -479,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +513,7 @@
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,8 +532,11 @@
       <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -534,8 +555,11 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -554,8 +578,11 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -574,8 +601,11 @@
       <c r="F4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -594,8 +624,11 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -614,8 +647,11 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -634,8 +670,11 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -654,8 +693,11 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -674,8 +716,11 @@
       <c r="F9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -694,8 +739,11 @@
       <c r="F10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -714,8 +762,11 @@
       <c r="F11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -734,8 +785,11 @@
       <c r="F12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -754,8 +808,11 @@
       <c r="F13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -774,8 +831,11 @@
       <c r="F14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -794,8 +854,11 @@
       <c r="F15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -814,8 +877,11 @@
       <c r="F16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -834,8 +900,11 @@
       <c r="F17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -854,8 +923,11 @@
       <c r="F18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -874,8 +946,11 @@
       <c r="F19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -894,8 +969,11 @@
       <c r="F20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -914,8 +992,11 @@
       <c r="F21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -934,8 +1015,11 @@
       <c r="F22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -954,8 +1038,11 @@
       <c r="F23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -974,8 +1061,11 @@
       <c r="F24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -994,8 +1084,11 @@
       <c r="F25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1014,8 +1107,11 @@
       <c r="F26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1034,8 +1130,11 @@
       <c r="F27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1054,8 +1153,11 @@
       <c r="F28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1074,8 +1176,11 @@
       <c r="F29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1094,8 +1199,11 @@
       <c r="F30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -1114,8 +1222,11 @@
       <c r="F31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1134,8 +1245,11 @@
       <c r="F32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -1154,8 +1268,11 @@
       <c r="F33" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1174,8 +1291,11 @@
       <c r="F34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1194,8 +1314,11 @@
       <c r="F35" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1214,8 +1337,11 @@
       <c r="F36" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1234,8 +1360,11 @@
       <c r="F37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1254,8 +1383,11 @@
       <c r="F38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1274,8 +1406,11 @@
       <c r="F39" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1294,8 +1429,11 @@
       <c r="F40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1314,8 +1452,11 @@
       <c r="F41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1334,8 +1475,11 @@
       <c r="F42" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1354,8 +1498,11 @@
       <c r="F43" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1374,8 +1521,11 @@
       <c r="F44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1394,8 +1544,11 @@
       <c r="F45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1414,8 +1567,11 @@
       <c r="F46" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1434,8 +1590,11 @@
       <c r="F47" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1454,8 +1613,11 @@
       <c r="F48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1474,8 +1636,11 @@
       <c r="F49" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1494,8 +1659,11 @@
       <c r="F50" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1514,8 +1682,11 @@
       <c r="F51" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1534,8 +1705,11 @@
       <c r="F52" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1554,8 +1728,11 @@
       <c r="F53" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1574,8 +1751,11 @@
       <c r="F54" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1594,8 +1774,11 @@
       <c r="F55" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1614,8 +1797,11 @@
       <c r="F56" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1634,8 +1820,11 @@
       <c r="F57" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1654,8 +1843,11 @@
       <c r="F58" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1674,8 +1866,11 @@
       <c r="F59" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1694,8 +1889,11 @@
       <c r="F60" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1714,8 +1912,11 @@
       <c r="F61" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1734,8 +1935,11 @@
       <c r="F62" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1754,8 +1958,11 @@
       <c r="F63" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -1774,8 +1981,11 @@
       <c r="F64" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -1794,8 +2004,11 @@
       <c r="F65" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -1814,8 +2027,11 @@
       <c r="F66" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -1834,8 +2050,11 @@
       <c r="F67" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -1854,8 +2073,11 @@
       <c r="F68" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -1874,8 +2096,11 @@
       <c r="F69" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -1894,8 +2119,11 @@
       <c r="F70" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -1914,8 +2142,12 @@
       <c r="F71" t="s">
         <v>23</v>
       </c>
+      <c r="G71" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correção de faixas etárias
</commit_message>
<xml_diff>
--- a/planos_de_saude_unificado.xlsx
+++ b/planos_de_saude_unificado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Torres\Documents\IDPB\cotacao-plano-saude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10700135-7D4B-4FC6-8EB7-5585839256B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD612CAA-A77B-4161-8087-B96E15AB6A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="46">
   <si>
     <t>Empresa</t>
   </si>
@@ -148,9 +148,6 @@
     <t>54 - 58</t>
   </si>
   <si>
-    <t>59 ou +</t>
-  </si>
-  <si>
     <t>SB Saúde</t>
   </si>
   <si>
@@ -225,13 +222,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3180,1583 +3175,1463 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C102" s="2" t="s">
+      <c r="A102" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" t="s">
         <v>32</v>
       </c>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2">
+      <c r="E102">
         <v>295.92</v>
       </c>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H102" s="2" t="s">
+      <c r="G102" t="s">
+        <v>33</v>
+      </c>
+      <c r="H102" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C103" s="2" t="s">
+      <c r="A103" t="s">
+        <v>31</v>
+      </c>
+      <c r="B103" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" t="s">
         <v>34</v>
       </c>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2">
+      <c r="E103">
         <v>378.77</v>
       </c>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H103" s="2" t="s">
+      <c r="G103" t="s">
+        <v>33</v>
+      </c>
+      <c r="H103" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C104" s="2" t="s">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" t="s">
         <v>35</v>
       </c>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2">
+      <c r="E104">
         <v>402.44</v>
       </c>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H104" s="2" t="s">
+      <c r="G104" t="s">
+        <v>33</v>
+      </c>
+      <c r="H104" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C105" s="2" t="s">
+      <c r="A105" t="s">
+        <v>31</v>
+      </c>
+      <c r="B105" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" t="s">
         <v>36</v>
       </c>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2">
+      <c r="E105">
         <v>414.23</v>
       </c>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H105" s="2" t="s">
+      <c r="G105" t="s">
+        <v>33</v>
+      </c>
+      <c r="H105" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C106" s="2" t="s">
+      <c r="A106" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" t="s">
         <v>37</v>
       </c>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2">
+      <c r="E106">
         <v>452.7</v>
       </c>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H106" s="2" t="s">
+      <c r="G106" t="s">
+        <v>33</v>
+      </c>
+      <c r="H106" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C107" s="2" t="s">
+      <c r="A107" t="s">
+        <v>31</v>
+      </c>
+      <c r="B107" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" t="s">
         <v>38</v>
       </c>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2">
+      <c r="E107">
         <v>517.79999999999995</v>
       </c>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H107" s="2" t="s">
+      <c r="G107" t="s">
+        <v>33</v>
+      </c>
+      <c r="H107" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C108" s="2" t="s">
+      <c r="A108" t="s">
+        <v>31</v>
+      </c>
+      <c r="B108" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" t="s">
         <v>39</v>
       </c>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2">
+      <c r="E108">
         <v>724.9</v>
       </c>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H108" s="2" t="s">
+      <c r="G108" t="s">
+        <v>33</v>
+      </c>
+      <c r="H108" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C109" s="2" t="s">
+      <c r="A109" t="s">
+        <v>31</v>
+      </c>
+      <c r="B109" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" t="s">
         <v>40</v>
       </c>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2">
+      <c r="E109">
         <v>970.51</v>
       </c>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H109" s="2" t="s">
+      <c r="G109" t="s">
+        <v>33</v>
+      </c>
+      <c r="H109" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C110" s="2" t="s">
+      <c r="A110" t="s">
+        <v>31</v>
+      </c>
+      <c r="B110" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" t="s">
         <v>41</v>
       </c>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2">
+      <c r="E110">
         <v>1088.9000000000001</v>
       </c>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H110" s="2" t="s">
+      <c r="G110" t="s">
+        <v>33</v>
+      </c>
+      <c r="H110" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C111" s="3" t="s">
+      <c r="A111" t="s">
+        <v>31</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111" t="s">
         <v>16</v>
       </c>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2">
+      <c r="E111">
         <v>1775.35</v>
       </c>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H111" s="2" t="s">
+      <c r="G111" t="s">
+        <v>33</v>
+      </c>
+      <c r="H111" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C112" s="2" t="s">
+      <c r="A112" t="s">
+        <v>31</v>
+      </c>
+      <c r="B112" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112" t="s">
         <v>32</v>
       </c>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2">
+      <c r="E112">
         <v>262.33999999999997</v>
       </c>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H112" s="2" t="s">
+      <c r="G112" t="s">
+        <v>33</v>
+      </c>
+      <c r="H112" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C113" s="2" t="s">
+      <c r="A113" t="s">
+        <v>31</v>
+      </c>
+      <c r="B113" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" t="s">
         <v>34</v>
       </c>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2">
+      <c r="E113">
         <v>297.56</v>
       </c>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H113" s="2" t="s">
+      <c r="G113" t="s">
+        <v>33</v>
+      </c>
+      <c r="H113" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C114" s="2" t="s">
+      <c r="A114" t="s">
+        <v>31</v>
+      </c>
+      <c r="B114" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114" t="s">
         <v>35</v>
       </c>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2">
+      <c r="E114">
         <v>327.25</v>
       </c>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H114" s="2" t="s">
+      <c r="G114" t="s">
+        <v>33</v>
+      </c>
+      <c r="H114" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C115" s="2" t="s">
+      <c r="A115" t="s">
+        <v>31</v>
+      </c>
+      <c r="B115" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2">
+      <c r="E115">
         <v>342.43</v>
       </c>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H115" s="2" t="s">
+      <c r="G115" t="s">
+        <v>33</v>
+      </c>
+      <c r="H115" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C116" s="2" t="s">
+      <c r="A116" t="s">
+        <v>31</v>
+      </c>
+      <c r="B116" t="s">
+        <v>17</v>
+      </c>
+      <c r="C116" t="s">
         <v>37</v>
       </c>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2">
+      <c r="E116">
         <v>407.46</v>
       </c>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H116" s="2" t="s">
+      <c r="G116" t="s">
+        <v>33</v>
+      </c>
+      <c r="H116" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C117" s="2" t="s">
+      <c r="A117" t="s">
+        <v>31</v>
+      </c>
+      <c r="B117" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117" t="s">
         <v>38</v>
       </c>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2">
+      <c r="E117">
         <v>476.74</v>
       </c>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H117" s="2" t="s">
+      <c r="G117" t="s">
+        <v>33</v>
+      </c>
+      <c r="H117" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C118" s="2" t="s">
+      <c r="A118" t="s">
+        <v>31</v>
+      </c>
+      <c r="B118" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118" t="s">
         <v>39</v>
       </c>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2">
+      <c r="E118">
         <v>643.61</v>
       </c>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H118" s="2" t="s">
+      <c r="G118" t="s">
+        <v>33</v>
+      </c>
+      <c r="H118" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C119" s="2" t="s">
+      <c r="A119" t="s">
+        <v>31</v>
+      </c>
+      <c r="B119" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" t="s">
         <v>40</v>
       </c>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2">
+      <c r="E119">
         <v>800.95</v>
       </c>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H119" s="2" t="s">
+      <c r="G119" t="s">
+        <v>33</v>
+      </c>
+      <c r="H119" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C120" s="2" t="s">
+      <c r="A120" t="s">
+        <v>31</v>
+      </c>
+      <c r="B120" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120" t="s">
         <v>41</v>
       </c>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2">
+      <c r="E120">
         <v>1121.3399999999999</v>
       </c>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H120" s="2" t="s">
+      <c r="G120" t="s">
+        <v>33</v>
+      </c>
+      <c r="H120" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C121" s="3" t="s">
+      <c r="A121" t="s">
+        <v>31</v>
+      </c>
+      <c r="B121" t="s">
+        <v>17</v>
+      </c>
+      <c r="C121" t="s">
         <v>16</v>
       </c>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2">
+      <c r="E121">
         <v>1570.97</v>
       </c>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H121" s="2" t="s">
+      <c r="G121" t="s">
+        <v>33</v>
+      </c>
+      <c r="H121" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C122" s="2" t="s">
+      <c r="A122" t="s">
+        <v>31</v>
+      </c>
+      <c r="B122" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" t="s">
         <v>32</v>
       </c>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2">
+      <c r="F122">
         <v>373.13</v>
       </c>
-      <c r="G122" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H122" s="2" t="s">
+      <c r="G122" t="s">
+        <v>33</v>
+      </c>
+      <c r="H122" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C123" s="2" t="s">
+      <c r="A123" t="s">
+        <v>31</v>
+      </c>
+      <c r="B123" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" t="s">
         <v>34</v>
       </c>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2">
+      <c r="F123">
         <v>442.9</v>
       </c>
-      <c r="G123" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H123" s="2" t="s">
+      <c r="G123" t="s">
+        <v>33</v>
+      </c>
+      <c r="H123" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C124" s="2" t="s">
+      <c r="A124" t="s">
+        <v>31</v>
+      </c>
+      <c r="B124" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124" t="s">
         <v>35</v>
       </c>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2">
+      <c r="F124">
         <v>531.48</v>
       </c>
-      <c r="G124" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H124" s="2" t="s">
+      <c r="G124" t="s">
+        <v>33</v>
+      </c>
+      <c r="H124" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C125" s="2" t="s">
+      <c r="A125" t="s">
+        <v>31</v>
+      </c>
+      <c r="B125" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" t="s">
         <v>36</v>
       </c>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2">
+      <c r="F125">
         <v>593.67999999999995</v>
       </c>
-      <c r="G125" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H125" s="2" t="s">
+      <c r="G125" t="s">
+        <v>33</v>
+      </c>
+      <c r="H125" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C126" s="2" t="s">
+      <c r="A126" t="s">
+        <v>31</v>
+      </c>
+      <c r="B126" t="s">
+        <v>17</v>
+      </c>
+      <c r="C126" t="s">
         <v>37</v>
       </c>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2">
+      <c r="F126">
         <v>664.91</v>
       </c>
-      <c r="G126" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H126" s="2" t="s">
+      <c r="G126" t="s">
+        <v>33</v>
+      </c>
+      <c r="H126" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C127" s="2" t="s">
+      <c r="A127" t="s">
+        <v>31</v>
+      </c>
+      <c r="B127" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" t="s">
         <v>38</v>
       </c>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2">
+      <c r="F127">
         <v>819.96</v>
       </c>
-      <c r="G127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H127" s="2" t="s">
+      <c r="G127" t="s">
+        <v>33</v>
+      </c>
+      <c r="H127" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C128" s="2" t="s">
+      <c r="A128" t="s">
+        <v>31</v>
+      </c>
+      <c r="B128" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" t="s">
         <v>39</v>
       </c>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2">
+      <c r="F128">
         <v>914.02</v>
       </c>
-      <c r="G128" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H128" s="2" t="s">
+      <c r="G128" t="s">
+        <v>33</v>
+      </c>
+      <c r="H128" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C129" s="2" t="s">
+      <c r="A129" t="s">
+        <v>31</v>
+      </c>
+      <c r="B129" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" t="s">
         <v>40</v>
       </c>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2">
+      <c r="F129">
         <v>1269.1199999999999</v>
       </c>
-      <c r="G129" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H129" s="2" t="s">
+      <c r="G129" t="s">
+        <v>33</v>
+      </c>
+      <c r="H129" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C130" s="2" t="s">
+      <c r="A130" t="s">
+        <v>31</v>
+      </c>
+      <c r="B130" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130" t="s">
         <v>41</v>
       </c>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
-      <c r="F130" s="2">
+      <c r="F130">
         <v>1785.8</v>
       </c>
-      <c r="G130" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H130" s="2" t="s">
+      <c r="G130" t="s">
+        <v>33</v>
+      </c>
+      <c r="H130" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C131" s="3" t="s">
+      <c r="A131" t="s">
+        <v>31</v>
+      </c>
+      <c r="B131" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" t="s">
         <v>16</v>
       </c>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2">
+      <c r="F131">
         <v>2234.34</v>
       </c>
-      <c r="G131" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H131" s="2" t="s">
+      <c r="G131" t="s">
+        <v>33</v>
+      </c>
+      <c r="H131" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C132" s="2" t="s">
+      <c r="A132" t="s">
+        <v>31</v>
+      </c>
+      <c r="B132" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132" t="s">
         <v>32</v>
       </c>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2">
+      <c r="F132">
         <v>354.17</v>
       </c>
-      <c r="G132" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H132" s="2" t="s">
+      <c r="G132" t="s">
+        <v>33</v>
+      </c>
+      <c r="H132" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C133" s="2" t="s">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+      <c r="B133" t="s">
+        <v>17</v>
+      </c>
+      <c r="C133" t="s">
         <v>34</v>
       </c>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2">
+      <c r="F133">
         <v>401.72</v>
       </c>
-      <c r="G133" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H133" s="2" t="s">
+      <c r="G133" t="s">
+        <v>33</v>
+      </c>
+      <c r="H133" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C134" s="2" t="s">
+      <c r="A134" t="s">
+        <v>31</v>
+      </c>
+      <c r="B134" t="s">
+        <v>17</v>
+      </c>
+      <c r="C134" t="s">
         <v>35</v>
       </c>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2">
+      <c r="F134">
         <v>441.8</v>
       </c>
-      <c r="G134" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H134" s="2" t="s">
+      <c r="G134" t="s">
+        <v>33</v>
+      </c>
+      <c r="H134" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C135" s="2" t="s">
+      <c r="A135" t="s">
+        <v>31</v>
+      </c>
+      <c r="B135" t="s">
+        <v>17</v>
+      </c>
+      <c r="C135" t="s">
         <v>36</v>
       </c>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2">
+      <c r="F135">
         <v>462.29</v>
       </c>
-      <c r="G135" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H135" s="2" t="s">
+      <c r="G135" t="s">
+        <v>33</v>
+      </c>
+      <c r="H135" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C136" s="2" t="s">
+      <c r="A136" t="s">
+        <v>31</v>
+      </c>
+      <c r="B136" t="s">
+        <v>17</v>
+      </c>
+      <c r="C136" t="s">
         <v>37</v>
       </c>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2">
+      <c r="F136">
         <v>550.1</v>
       </c>
-      <c r="G136" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H136" s="2" t="s">
+      <c r="G136" t="s">
+        <v>33</v>
+      </c>
+      <c r="H136" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C137" s="2" t="s">
+      <c r="A137" t="s">
+        <v>31</v>
+      </c>
+      <c r="B137" t="s">
+        <v>17</v>
+      </c>
+      <c r="C137" t="s">
         <v>38</v>
       </c>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2">
+      <c r="F137">
         <v>643.61</v>
       </c>
-      <c r="G137" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H137" s="2" t="s">
+      <c r="G137" t="s">
+        <v>33</v>
+      </c>
+      <c r="H137" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C138" s="2" t="s">
+      <c r="A138" t="s">
+        <v>31</v>
+      </c>
+      <c r="B138" t="s">
+        <v>17</v>
+      </c>
+      <c r="C138" t="s">
         <v>39</v>
       </c>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2">
+      <c r="F138">
         <v>868.89</v>
       </c>
-      <c r="G138" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H138" s="2" t="s">
+      <c r="G138" t="s">
+        <v>33</v>
+      </c>
+      <c r="H138" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A139" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C139" s="2" t="s">
+      <c r="A139" t="s">
+        <v>31</v>
+      </c>
+      <c r="B139" t="s">
+        <v>17</v>
+      </c>
+      <c r="C139" t="s">
         <v>40</v>
       </c>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2">
+      <c r="F139">
         <v>1081.32</v>
       </c>
-      <c r="G139" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H139" s="2" t="s">
+      <c r="G139" t="s">
+        <v>33</v>
+      </c>
+      <c r="H139" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C140" s="2" t="s">
+      <c r="A140" t="s">
+        <v>31</v>
+      </c>
+      <c r="B140" t="s">
+        <v>17</v>
+      </c>
+      <c r="C140" t="s">
         <v>41</v>
       </c>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2">
+      <c r="F140">
         <v>1513.85</v>
       </c>
-      <c r="G140" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H140" s="2" t="s">
+      <c r="G140" t="s">
+        <v>33</v>
+      </c>
+      <c r="H140" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C141" s="2" t="s">
+      <c r="A141" t="s">
+        <v>31</v>
+      </c>
+      <c r="B141" t="s">
+        <v>17</v>
+      </c>
+      <c r="C141" t="s">
+        <v>16</v>
+      </c>
+      <c r="F141">
+        <v>2120.81</v>
+      </c>
+      <c r="G141" t="s">
+        <v>33</v>
+      </c>
+      <c r="H141" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>31</v>
+      </c>
+      <c r="B142" t="s">
+        <v>17</v>
+      </c>
+      <c r="C142" t="s">
+        <v>32</v>
+      </c>
+      <c r="F142">
+        <v>594.27</v>
+      </c>
+      <c r="G142" t="s">
+        <v>33</v>
+      </c>
+      <c r="H142" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>31</v>
+      </c>
+      <c r="B143" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" t="s">
+        <v>34</v>
+      </c>
+      <c r="F143">
+        <v>760.63</v>
+      </c>
+      <c r="G143" t="s">
+        <v>33</v>
+      </c>
+      <c r="H143" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>31</v>
+      </c>
+      <c r="B144" t="s">
+        <v>17</v>
+      </c>
+      <c r="C144" t="s">
+        <v>35</v>
+      </c>
+      <c r="F144">
+        <v>808.05</v>
+      </c>
+      <c r="G144" t="s">
+        <v>33</v>
+      </c>
+      <c r="H144" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>31</v>
+      </c>
+      <c r="B145" t="s">
+        <v>17</v>
+      </c>
+      <c r="C145" t="s">
+        <v>36</v>
+      </c>
+      <c r="F145">
+        <v>831.82</v>
+      </c>
+      <c r="G145" t="s">
+        <v>33</v>
+      </c>
+      <c r="H145" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>31</v>
+      </c>
+      <c r="B146" t="s">
+        <v>17</v>
+      </c>
+      <c r="C146" t="s">
+        <v>37</v>
+      </c>
+      <c r="F146">
+        <v>909.05</v>
+      </c>
+      <c r="G146" t="s">
+        <v>33</v>
+      </c>
+      <c r="H146" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>31</v>
+      </c>
+      <c r="B147" t="s">
+        <v>17</v>
+      </c>
+      <c r="C147" t="s">
+        <v>38</v>
+      </c>
+      <c r="F147">
+        <v>1039.76</v>
+      </c>
+      <c r="G147" t="s">
+        <v>33</v>
+      </c>
+      <c r="H147" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>31</v>
+      </c>
+      <c r="B148" t="s">
+        <v>17</v>
+      </c>
+      <c r="C148" t="s">
+        <v>39</v>
+      </c>
+      <c r="F148">
+        <v>1455.73</v>
+      </c>
+      <c r="G148" t="s">
+        <v>33</v>
+      </c>
+      <c r="H148" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>31</v>
+      </c>
+      <c r="B149" t="s">
+        <v>17</v>
+      </c>
+      <c r="C149" t="s">
+        <v>40</v>
+      </c>
+      <c r="F149">
+        <v>1948.96</v>
+      </c>
+      <c r="G149" t="s">
+        <v>33</v>
+      </c>
+      <c r="H149" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>31</v>
+      </c>
+      <c r="B150" t="s">
+        <v>17</v>
+      </c>
+      <c r="C150" t="s">
+        <v>41</v>
+      </c>
+      <c r="F150">
+        <v>2186.75</v>
+      </c>
+      <c r="G150" t="s">
+        <v>33</v>
+      </c>
+      <c r="H150" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>31</v>
+      </c>
+      <c r="B151" t="s">
+        <v>17</v>
+      </c>
+      <c r="C151" t="s">
+        <v>16</v>
+      </c>
+      <c r="F151">
+        <v>3565.09</v>
+      </c>
+      <c r="G151" t="s">
+        <v>33</v>
+      </c>
+      <c r="H151" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>31</v>
+      </c>
+      <c r="B152" t="s">
+        <v>17</v>
+      </c>
+      <c r="C152" t="s">
+        <v>32</v>
+      </c>
+      <c r="F152">
+        <v>482.31</v>
+      </c>
+      <c r="G152" t="s">
+        <v>33</v>
+      </c>
+      <c r="H152" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>31</v>
+      </c>
+      <c r="B153" t="s">
+        <v>17</v>
+      </c>
+      <c r="C153" t="s">
+        <v>34</v>
+      </c>
+      <c r="F153">
+        <v>547.26</v>
+      </c>
+      <c r="G153" t="s">
+        <v>33</v>
+      </c>
+      <c r="H153" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>31</v>
+      </c>
+      <c r="B154" t="s">
+        <v>17</v>
+      </c>
+      <c r="C154" t="s">
+        <v>35</v>
+      </c>
+      <c r="F154">
+        <v>601.89</v>
+      </c>
+      <c r="G154" t="s">
+        <v>33</v>
+      </c>
+      <c r="H154" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>31</v>
+      </c>
+      <c r="B155" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155" t="s">
+        <v>36</v>
+      </c>
+      <c r="F155">
+        <v>629.79999999999995</v>
+      </c>
+      <c r="G155" t="s">
+        <v>33</v>
+      </c>
+      <c r="H155" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>31</v>
+      </c>
+      <c r="B156" t="s">
+        <v>17</v>
+      </c>
+      <c r="C156" t="s">
+        <v>37</v>
+      </c>
+      <c r="F156">
+        <v>749.41</v>
+      </c>
+      <c r="G156" t="s">
+        <v>33</v>
+      </c>
+      <c r="H156" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>31</v>
+      </c>
+      <c r="B157" t="s">
+        <v>17</v>
+      </c>
+      <c r="C157" t="s">
+        <v>38</v>
+      </c>
+      <c r="F157">
+        <v>876.81</v>
+      </c>
+      <c r="G157" t="s">
+        <v>33</v>
+      </c>
+      <c r="H157" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>31</v>
+      </c>
+      <c r="B158" t="s">
+        <v>17</v>
+      </c>
+      <c r="C158" t="s">
+        <v>39</v>
+      </c>
+      <c r="F158">
+        <v>1183.72</v>
+      </c>
+      <c r="G158" t="s">
+        <v>33</v>
+      </c>
+      <c r="H158" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>31</v>
+      </c>
+      <c r="B159" t="s">
+        <v>17</v>
+      </c>
+      <c r="C159" t="s">
+        <v>40</v>
+      </c>
+      <c r="F159">
+        <v>1473.12</v>
+      </c>
+      <c r="G159" t="s">
+        <v>33</v>
+      </c>
+      <c r="H159" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>31</v>
+      </c>
+      <c r="B160" t="s">
+        <v>17</v>
+      </c>
+      <c r="C160" t="s">
+        <v>41</v>
+      </c>
+      <c r="F160">
+        <v>2062.36</v>
+      </c>
+      <c r="G160" t="s">
+        <v>33</v>
+      </c>
+      <c r="H160" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>31</v>
+      </c>
+      <c r="B161" t="s">
+        <v>17</v>
+      </c>
+      <c r="C161" t="s">
+        <v>16</v>
+      </c>
+      <c r="F161">
+        <v>2893.86</v>
+      </c>
+      <c r="G161" t="s">
+        <v>33</v>
+      </c>
+      <c r="H161" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>42</v>
       </c>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2">
-        <v>2120.81</v>
-      </c>
-      <c r="G141" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H141" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A142" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2">
-        <v>594.27</v>
-      </c>
-      <c r="G142" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H142" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A143" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2">
-        <v>760.63</v>
-      </c>
-      <c r="G143" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H143" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2">
-        <v>808.05</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H144" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="F145" s="2">
-        <v>831.82</v>
-      </c>
-      <c r="G145" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H145" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D146" s="2"/>
-      <c r="E146" s="2"/>
-      <c r="F146" s="2">
-        <v>909.05</v>
-      </c>
-      <c r="G146" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H146" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2">
-        <v>1039.76</v>
-      </c>
-      <c r="G147" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H147" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A148" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2">
-        <v>1455.73</v>
-      </c>
-      <c r="G148" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A149" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
-      <c r="F149" s="2">
-        <v>1948.96</v>
-      </c>
-      <c r="G149" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2">
-        <v>2186.75</v>
-      </c>
-      <c r="G150" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A151" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C151" s="3" t="s">
+      <c r="B162" t="s">
+        <v>43</v>
+      </c>
+      <c r="C162" t="s">
+        <v>45</v>
+      </c>
+      <c r="D162" t="s">
+        <v>24</v>
+      </c>
+      <c r="E162">
+        <v>174.49</v>
+      </c>
+      <c r="F162">
+        <v>255.42</v>
+      </c>
+      <c r="G162" t="s">
+        <v>20</v>
+      </c>
+      <c r="H162" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>42</v>
+      </c>
+      <c r="B163" t="s">
+        <v>43</v>
+      </c>
+      <c r="C163" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" t="s">
+        <v>24</v>
+      </c>
+      <c r="E163">
+        <v>225.69</v>
+      </c>
+      <c r="F163">
+        <v>369.98</v>
+      </c>
+      <c r="G163" t="s">
+        <v>20</v>
+      </c>
+      <c r="H163" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>42</v>
+      </c>
+      <c r="B164" t="s">
+        <v>43</v>
+      </c>
+      <c r="C164" t="s">
+        <v>9</v>
+      </c>
+      <c r="D164" t="s">
+        <v>24</v>
+      </c>
+      <c r="E164">
+        <v>252.76</v>
+      </c>
+      <c r="F164">
+        <v>406.58</v>
+      </c>
+      <c r="G164" t="s">
+        <v>20</v>
+      </c>
+      <c r="H164" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>42</v>
+      </c>
+      <c r="B165" t="s">
+        <v>43</v>
+      </c>
+      <c r="C165" t="s">
+        <v>10</v>
+      </c>
+      <c r="D165" t="s">
+        <v>24</v>
+      </c>
+      <c r="E165">
+        <v>283.08</v>
+      </c>
+      <c r="F165">
+        <v>414.43</v>
+      </c>
+      <c r="G165" t="s">
+        <v>20</v>
+      </c>
+      <c r="H165" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>42</v>
+      </c>
+      <c r="B166" t="s">
+        <v>43</v>
+      </c>
+      <c r="C166" t="s">
+        <v>11</v>
+      </c>
+      <c r="D166" t="s">
+        <v>24</v>
+      </c>
+      <c r="E166">
+        <v>318.67</v>
+      </c>
+      <c r="F166">
+        <v>466.5</v>
+      </c>
+      <c r="G166" t="s">
+        <v>20</v>
+      </c>
+      <c r="H166" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>42</v>
+      </c>
+      <c r="B167" t="s">
+        <v>43</v>
+      </c>
+      <c r="C167" t="s">
+        <v>12</v>
+      </c>
+      <c r="D167" t="s">
+        <v>24</v>
+      </c>
+      <c r="E167">
+        <v>359.24</v>
+      </c>
+      <c r="F167">
+        <v>525.9</v>
+      </c>
+      <c r="G167" t="s">
+        <v>20</v>
+      </c>
+      <c r="H167" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>42</v>
+      </c>
+      <c r="B168" t="s">
+        <v>43</v>
+      </c>
+      <c r="C168" t="s">
+        <v>13</v>
+      </c>
+      <c r="D168" t="s">
+        <v>24</v>
+      </c>
+      <c r="E168">
+        <v>449.07</v>
+      </c>
+      <c r="F168">
+        <v>657.38</v>
+      </c>
+      <c r="G168" t="s">
+        <v>20</v>
+      </c>
+      <c r="H168" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>42</v>
+      </c>
+      <c r="B169" t="s">
+        <v>43</v>
+      </c>
+      <c r="C169" t="s">
+        <v>14</v>
+      </c>
+      <c r="D169" t="s">
+        <v>24</v>
+      </c>
+      <c r="E169">
+        <v>538.88</v>
+      </c>
+      <c r="F169">
+        <v>788.85</v>
+      </c>
+      <c r="G169" t="s">
+        <v>20</v>
+      </c>
+      <c r="H169" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>42</v>
+      </c>
+      <c r="B170" t="s">
+        <v>43</v>
+      </c>
+      <c r="C170" t="s">
+        <v>15</v>
+      </c>
+      <c r="D170" t="s">
+        <v>24</v>
+      </c>
+      <c r="E170">
+        <v>733.84</v>
+      </c>
+      <c r="F170">
+        <v>1074.25</v>
+      </c>
+      <c r="G170" t="s">
+        <v>20</v>
+      </c>
+      <c r="H170" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>42</v>
+      </c>
+      <c r="B171" t="s">
+        <v>43</v>
+      </c>
+      <c r="C171" t="s">
         <v>16</v>
       </c>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="2">
-        <v>3565.09</v>
-      </c>
-      <c r="G151" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H151" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2">
-        <v>482.31</v>
-      </c>
-      <c r="G152" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H152" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
-      <c r="F153" s="2">
-        <v>547.26</v>
-      </c>
-      <c r="G153" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H153" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A154" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2">
-        <v>601.89</v>
-      </c>
-      <c r="G154" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H154" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A155" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2">
-        <v>629.79999999999995</v>
-      </c>
-      <c r="G155" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H155" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A156" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2"/>
-      <c r="F156" s="2">
-        <v>749.41</v>
-      </c>
-      <c r="G156" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H156" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A157" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D157" s="2"/>
-      <c r="E157" s="2"/>
-      <c r="F157" s="2">
-        <v>876.81</v>
-      </c>
-      <c r="G157" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H157" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A158" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
-      <c r="F158" s="2">
-        <v>1183.72</v>
-      </c>
-      <c r="G158" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H158" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A159" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2"/>
-      <c r="F159" s="2">
-        <v>1473.12</v>
-      </c>
-      <c r="G159" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H159" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A160" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2">
-        <v>2062.36</v>
-      </c>
-      <c r="G160" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H160" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2">
-        <v>2893.86</v>
-      </c>
-      <c r="G161" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H161" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A162" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B162" s="3" t="s">
+      <c r="D171" t="s">
+        <v>24</v>
+      </c>
+      <c r="E171">
+        <v>1039.8900000000001</v>
+      </c>
+      <c r="F171">
+        <v>1522.23</v>
+      </c>
+      <c r="G171" t="s">
+        <v>20</v>
+      </c>
+      <c r="H171" t="s">
         <v>44</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E162" s="3">
-        <v>174.49</v>
-      </c>
-      <c r="F162" s="3">
-        <v>255.42</v>
-      </c>
-      <c r="G162" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H162" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A163" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E163" s="3">
-        <v>225.69</v>
-      </c>
-      <c r="F163" s="3">
-        <v>369.98</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H163" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A164" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E164" s="3">
-        <v>252.76</v>
-      </c>
-      <c r="F164" s="3">
-        <v>406.58</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H164" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A165" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D165" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E165" s="3">
-        <v>283.08</v>
-      </c>
-      <c r="F165" s="3">
-        <v>414.43</v>
-      </c>
-      <c r="G165" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H165" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A166" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E166" s="3">
-        <v>318.67</v>
-      </c>
-      <c r="F166" s="3">
-        <v>466.5</v>
-      </c>
-      <c r="G166" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H166" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A167" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D167" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E167" s="3">
-        <v>359.24</v>
-      </c>
-      <c r="F167" s="3">
-        <v>525.9</v>
-      </c>
-      <c r="G167" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H167" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D168" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E168" s="3">
-        <v>449.07</v>
-      </c>
-      <c r="F168" s="3">
-        <v>657.38</v>
-      </c>
-      <c r="G168" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H168" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D169" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E169" s="3">
-        <v>538.88</v>
-      </c>
-      <c r="F169" s="3">
-        <v>788.85</v>
-      </c>
-      <c r="G169" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H169" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E170" s="3">
-        <v>733.84</v>
-      </c>
-      <c r="F170" s="3">
-        <v>1074.25</v>
-      </c>
-      <c r="G170" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H170" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A171" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E171" s="3">
-        <v>1039.8900000000001</v>
-      </c>
-      <c r="F171" s="3">
-        <v>1522.23</v>
-      </c>
-      <c r="G171" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H171" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Colocando - em valores vazios
</commit_message>
<xml_diff>
--- a/planos_de_saude_unificado.xlsx
+++ b/planos_de_saude_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Torres\Documents\IDPB\cotacao-plano-saude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD612CAA-A77B-4161-8087-B96E15AB6A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E91FA92-95C6-458E-9306-E841D4FFBDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="46">
   <si>
     <t>Empresa</t>
   </si>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141:E161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3184,9 +3184,15 @@
       <c r="C102" t="s">
         <v>32</v>
       </c>
+      <c r="D102" t="s">
+        <v>24</v>
+      </c>
       <c r="E102">
         <v>295.92</v>
       </c>
+      <c r="F102" t="s">
+        <v>24</v>
+      </c>
       <c r="G102" t="s">
         <v>33</v>
       </c>
@@ -3204,9 +3210,15 @@
       <c r="C103" t="s">
         <v>34</v>
       </c>
+      <c r="D103" t="s">
+        <v>24</v>
+      </c>
       <c r="E103">
         <v>378.77</v>
       </c>
+      <c r="F103" t="s">
+        <v>24</v>
+      </c>
       <c r="G103" t="s">
         <v>33</v>
       </c>
@@ -3224,9 +3236,15 @@
       <c r="C104" t="s">
         <v>35</v>
       </c>
+      <c r="D104" t="s">
+        <v>24</v>
+      </c>
       <c r="E104">
         <v>402.44</v>
       </c>
+      <c r="F104" t="s">
+        <v>24</v>
+      </c>
       <c r="G104" t="s">
         <v>33</v>
       </c>
@@ -3244,9 +3262,15 @@
       <c r="C105" t="s">
         <v>36</v>
       </c>
+      <c r="D105" t="s">
+        <v>24</v>
+      </c>
       <c r="E105">
         <v>414.23</v>
       </c>
+      <c r="F105" t="s">
+        <v>24</v>
+      </c>
       <c r="G105" t="s">
         <v>33</v>
       </c>
@@ -3264,9 +3288,15 @@
       <c r="C106" t="s">
         <v>37</v>
       </c>
+      <c r="D106" t="s">
+        <v>24</v>
+      </c>
       <c r="E106">
         <v>452.7</v>
       </c>
+      <c r="F106" t="s">
+        <v>24</v>
+      </c>
       <c r="G106" t="s">
         <v>33</v>
       </c>
@@ -3284,9 +3314,15 @@
       <c r="C107" t="s">
         <v>38</v>
       </c>
+      <c r="D107" t="s">
+        <v>24</v>
+      </c>
       <c r="E107">
         <v>517.79999999999995</v>
       </c>
+      <c r="F107" t="s">
+        <v>24</v>
+      </c>
       <c r="G107" t="s">
         <v>33</v>
       </c>
@@ -3304,9 +3340,15 @@
       <c r="C108" t="s">
         <v>39</v>
       </c>
+      <c r="D108" t="s">
+        <v>24</v>
+      </c>
       <c r="E108">
         <v>724.9</v>
       </c>
+      <c r="F108" t="s">
+        <v>24</v>
+      </c>
       <c r="G108" t="s">
         <v>33</v>
       </c>
@@ -3324,9 +3366,15 @@
       <c r="C109" t="s">
         <v>40</v>
       </c>
+      <c r="D109" t="s">
+        <v>24</v>
+      </c>
       <c r="E109">
         <v>970.51</v>
       </c>
+      <c r="F109" t="s">
+        <v>24</v>
+      </c>
       <c r="G109" t="s">
         <v>33</v>
       </c>
@@ -3344,9 +3392,15 @@
       <c r="C110" t="s">
         <v>41</v>
       </c>
+      <c r="D110" t="s">
+        <v>24</v>
+      </c>
       <c r="E110">
         <v>1088.9000000000001</v>
       </c>
+      <c r="F110" t="s">
+        <v>24</v>
+      </c>
       <c r="G110" t="s">
         <v>33</v>
       </c>
@@ -3364,9 +3418,15 @@
       <c r="C111" t="s">
         <v>16</v>
       </c>
+      <c r="D111" t="s">
+        <v>24</v>
+      </c>
       <c r="E111">
         <v>1775.35</v>
       </c>
+      <c r="F111" t="s">
+        <v>24</v>
+      </c>
       <c r="G111" t="s">
         <v>33</v>
       </c>
@@ -3384,9 +3444,15 @@
       <c r="C112" t="s">
         <v>32</v>
       </c>
+      <c r="D112" t="s">
+        <v>24</v>
+      </c>
       <c r="E112">
         <v>262.33999999999997</v>
       </c>
+      <c r="F112" t="s">
+        <v>24</v>
+      </c>
       <c r="G112" t="s">
         <v>33</v>
       </c>
@@ -3404,9 +3470,15 @@
       <c r="C113" t="s">
         <v>34</v>
       </c>
+      <c r="D113" t="s">
+        <v>24</v>
+      </c>
       <c r="E113">
         <v>297.56</v>
       </c>
+      <c r="F113" t="s">
+        <v>24</v>
+      </c>
       <c r="G113" t="s">
         <v>33</v>
       </c>
@@ -3424,9 +3496,15 @@
       <c r="C114" t="s">
         <v>35</v>
       </c>
+      <c r="D114" t="s">
+        <v>24</v>
+      </c>
       <c r="E114">
         <v>327.25</v>
       </c>
+      <c r="F114" t="s">
+        <v>24</v>
+      </c>
       <c r="G114" t="s">
         <v>33</v>
       </c>
@@ -3444,9 +3522,15 @@
       <c r="C115" t="s">
         <v>36</v>
       </c>
+      <c r="D115" t="s">
+        <v>24</v>
+      </c>
       <c r="E115">
         <v>342.43</v>
       </c>
+      <c r="F115" t="s">
+        <v>24</v>
+      </c>
       <c r="G115" t="s">
         <v>33</v>
       </c>
@@ -3464,9 +3548,15 @@
       <c r="C116" t="s">
         <v>37</v>
       </c>
+      <c r="D116" t="s">
+        <v>24</v>
+      </c>
       <c r="E116">
         <v>407.46</v>
       </c>
+      <c r="F116" t="s">
+        <v>24</v>
+      </c>
       <c r="G116" t="s">
         <v>33</v>
       </c>
@@ -3484,9 +3574,15 @@
       <c r="C117" t="s">
         <v>38</v>
       </c>
+      <c r="D117" t="s">
+        <v>24</v>
+      </c>
       <c r="E117">
         <v>476.74</v>
       </c>
+      <c r="F117" t="s">
+        <v>24</v>
+      </c>
       <c r="G117" t="s">
         <v>33</v>
       </c>
@@ -3504,9 +3600,15 @@
       <c r="C118" t="s">
         <v>39</v>
       </c>
+      <c r="D118" t="s">
+        <v>24</v>
+      </c>
       <c r="E118">
         <v>643.61</v>
       </c>
+      <c r="F118" t="s">
+        <v>24</v>
+      </c>
       <c r="G118" t="s">
         <v>33</v>
       </c>
@@ -3524,9 +3626,15 @@
       <c r="C119" t="s">
         <v>40</v>
       </c>
+      <c r="D119" t="s">
+        <v>24</v>
+      </c>
       <c r="E119">
         <v>800.95</v>
       </c>
+      <c r="F119" t="s">
+        <v>24</v>
+      </c>
       <c r="G119" t="s">
         <v>33</v>
       </c>
@@ -3544,9 +3652,15 @@
       <c r="C120" t="s">
         <v>41</v>
       </c>
+      <c r="D120" t="s">
+        <v>24</v>
+      </c>
       <c r="E120">
         <v>1121.3399999999999</v>
       </c>
+      <c r="F120" t="s">
+        <v>24</v>
+      </c>
       <c r="G120" t="s">
         <v>33</v>
       </c>
@@ -3564,9 +3678,15 @@
       <c r="C121" t="s">
         <v>16</v>
       </c>
+      <c r="D121" t="s">
+        <v>24</v>
+      </c>
       <c r="E121">
         <v>1570.97</v>
       </c>
+      <c r="F121" t="s">
+        <v>24</v>
+      </c>
       <c r="G121" t="s">
         <v>33</v>
       </c>
@@ -3584,6 +3704,12 @@
       <c r="C122" t="s">
         <v>32</v>
       </c>
+      <c r="D122" t="s">
+        <v>24</v>
+      </c>
+      <c r="E122" t="s">
+        <v>24</v>
+      </c>
       <c r="F122">
         <v>373.13</v>
       </c>
@@ -3604,6 +3730,12 @@
       <c r="C123" t="s">
         <v>34</v>
       </c>
+      <c r="D123" t="s">
+        <v>24</v>
+      </c>
+      <c r="E123" t="s">
+        <v>24</v>
+      </c>
       <c r="F123">
         <v>442.9</v>
       </c>
@@ -3624,6 +3756,12 @@
       <c r="C124" t="s">
         <v>35</v>
       </c>
+      <c r="D124" t="s">
+        <v>24</v>
+      </c>
+      <c r="E124" t="s">
+        <v>24</v>
+      </c>
       <c r="F124">
         <v>531.48</v>
       </c>
@@ -3644,6 +3782,12 @@
       <c r="C125" t="s">
         <v>36</v>
       </c>
+      <c r="D125" t="s">
+        <v>24</v>
+      </c>
+      <c r="E125" t="s">
+        <v>24</v>
+      </c>
       <c r="F125">
         <v>593.67999999999995</v>
       </c>
@@ -3664,6 +3808,12 @@
       <c r="C126" t="s">
         <v>37</v>
       </c>
+      <c r="D126" t="s">
+        <v>24</v>
+      </c>
+      <c r="E126" t="s">
+        <v>24</v>
+      </c>
       <c r="F126">
         <v>664.91</v>
       </c>
@@ -3684,6 +3834,12 @@
       <c r="C127" t="s">
         <v>38</v>
       </c>
+      <c r="D127" t="s">
+        <v>24</v>
+      </c>
+      <c r="E127" t="s">
+        <v>24</v>
+      </c>
       <c r="F127">
         <v>819.96</v>
       </c>
@@ -3704,6 +3860,12 @@
       <c r="C128" t="s">
         <v>39</v>
       </c>
+      <c r="D128" t="s">
+        <v>24</v>
+      </c>
+      <c r="E128" t="s">
+        <v>24</v>
+      </c>
       <c r="F128">
         <v>914.02</v>
       </c>
@@ -3724,6 +3886,12 @@
       <c r="C129" t="s">
         <v>40</v>
       </c>
+      <c r="D129" t="s">
+        <v>24</v>
+      </c>
+      <c r="E129" t="s">
+        <v>24</v>
+      </c>
       <c r="F129">
         <v>1269.1199999999999</v>
       </c>
@@ -3744,6 +3912,12 @@
       <c r="C130" t="s">
         <v>41</v>
       </c>
+      <c r="D130" t="s">
+        <v>24</v>
+      </c>
+      <c r="E130" t="s">
+        <v>24</v>
+      </c>
       <c r="F130">
         <v>1785.8</v>
       </c>
@@ -3764,6 +3938,12 @@
       <c r="C131" t="s">
         <v>16</v>
       </c>
+      <c r="D131" t="s">
+        <v>24</v>
+      </c>
+      <c r="E131" t="s">
+        <v>24</v>
+      </c>
       <c r="F131">
         <v>2234.34</v>
       </c>
@@ -3784,6 +3964,12 @@
       <c r="C132" t="s">
         <v>32</v>
       </c>
+      <c r="D132" t="s">
+        <v>24</v>
+      </c>
+      <c r="E132" t="s">
+        <v>24</v>
+      </c>
       <c r="F132">
         <v>354.17</v>
       </c>
@@ -3804,6 +3990,12 @@
       <c r="C133" t="s">
         <v>34</v>
       </c>
+      <c r="D133" t="s">
+        <v>24</v>
+      </c>
+      <c r="E133" t="s">
+        <v>24</v>
+      </c>
       <c r="F133">
         <v>401.72</v>
       </c>
@@ -3824,6 +4016,12 @@
       <c r="C134" t="s">
         <v>35</v>
       </c>
+      <c r="D134" t="s">
+        <v>24</v>
+      </c>
+      <c r="E134" t="s">
+        <v>24</v>
+      </c>
       <c r="F134">
         <v>441.8</v>
       </c>
@@ -3844,6 +4042,12 @@
       <c r="C135" t="s">
         <v>36</v>
       </c>
+      <c r="D135" t="s">
+        <v>24</v>
+      </c>
+      <c r="E135" t="s">
+        <v>24</v>
+      </c>
       <c r="F135">
         <v>462.29</v>
       </c>
@@ -3864,6 +4068,12 @@
       <c r="C136" t="s">
         <v>37</v>
       </c>
+      <c r="D136" t="s">
+        <v>24</v>
+      </c>
+      <c r="E136" t="s">
+        <v>24</v>
+      </c>
       <c r="F136">
         <v>550.1</v>
       </c>
@@ -3884,6 +4094,12 @@
       <c r="C137" t="s">
         <v>38</v>
       </c>
+      <c r="D137" t="s">
+        <v>24</v>
+      </c>
+      <c r="E137" t="s">
+        <v>24</v>
+      </c>
       <c r="F137">
         <v>643.61</v>
       </c>
@@ -3904,6 +4120,12 @@
       <c r="C138" t="s">
         <v>39</v>
       </c>
+      <c r="D138" t="s">
+        <v>24</v>
+      </c>
+      <c r="E138" t="s">
+        <v>24</v>
+      </c>
       <c r="F138">
         <v>868.89</v>
       </c>
@@ -3924,6 +4146,12 @@
       <c r="C139" t="s">
         <v>40</v>
       </c>
+      <c r="D139" t="s">
+        <v>24</v>
+      </c>
+      <c r="E139" t="s">
+        <v>24</v>
+      </c>
       <c r="F139">
         <v>1081.32</v>
       </c>
@@ -3944,6 +4172,12 @@
       <c r="C140" t="s">
         <v>41</v>
       </c>
+      <c r="D140" t="s">
+        <v>24</v>
+      </c>
+      <c r="E140" t="s">
+        <v>24</v>
+      </c>
       <c r="F140">
         <v>1513.85</v>
       </c>
@@ -3964,6 +4198,12 @@
       <c r="C141" t="s">
         <v>16</v>
       </c>
+      <c r="D141" t="s">
+        <v>24</v>
+      </c>
+      <c r="E141" t="s">
+        <v>24</v>
+      </c>
       <c r="F141">
         <v>2120.81</v>
       </c>
@@ -3984,6 +4224,12 @@
       <c r="C142" t="s">
         <v>32</v>
       </c>
+      <c r="D142" t="s">
+        <v>24</v>
+      </c>
+      <c r="E142" t="s">
+        <v>24</v>
+      </c>
       <c r="F142">
         <v>594.27</v>
       </c>
@@ -4004,6 +4250,12 @@
       <c r="C143" t="s">
         <v>34</v>
       </c>
+      <c r="D143" t="s">
+        <v>24</v>
+      </c>
+      <c r="E143" t="s">
+        <v>24</v>
+      </c>
       <c r="F143">
         <v>760.63</v>
       </c>
@@ -4024,6 +4276,12 @@
       <c r="C144" t="s">
         <v>35</v>
       </c>
+      <c r="D144" t="s">
+        <v>24</v>
+      </c>
+      <c r="E144" t="s">
+        <v>24</v>
+      </c>
       <c r="F144">
         <v>808.05</v>
       </c>
@@ -4044,6 +4302,12 @@
       <c r="C145" t="s">
         <v>36</v>
       </c>
+      <c r="D145" t="s">
+        <v>24</v>
+      </c>
+      <c r="E145" t="s">
+        <v>24</v>
+      </c>
       <c r="F145">
         <v>831.82</v>
       </c>
@@ -4064,6 +4328,12 @@
       <c r="C146" t="s">
         <v>37</v>
       </c>
+      <c r="D146" t="s">
+        <v>24</v>
+      </c>
+      <c r="E146" t="s">
+        <v>24</v>
+      </c>
       <c r="F146">
         <v>909.05</v>
       </c>
@@ -4084,6 +4354,12 @@
       <c r="C147" t="s">
         <v>38</v>
       </c>
+      <c r="D147" t="s">
+        <v>24</v>
+      </c>
+      <c r="E147" t="s">
+        <v>24</v>
+      </c>
       <c r="F147">
         <v>1039.76</v>
       </c>
@@ -4104,6 +4380,12 @@
       <c r="C148" t="s">
         <v>39</v>
       </c>
+      <c r="D148" t="s">
+        <v>24</v>
+      </c>
+      <c r="E148" t="s">
+        <v>24</v>
+      </c>
       <c r="F148">
         <v>1455.73</v>
       </c>
@@ -4124,6 +4406,12 @@
       <c r="C149" t="s">
         <v>40</v>
       </c>
+      <c r="D149" t="s">
+        <v>24</v>
+      </c>
+      <c r="E149" t="s">
+        <v>24</v>
+      </c>
       <c r="F149">
         <v>1948.96</v>
       </c>
@@ -4144,6 +4432,12 @@
       <c r="C150" t="s">
         <v>41</v>
       </c>
+      <c r="D150" t="s">
+        <v>24</v>
+      </c>
+      <c r="E150" t="s">
+        <v>24</v>
+      </c>
       <c r="F150">
         <v>2186.75</v>
       </c>
@@ -4164,6 +4458,12 @@
       <c r="C151" t="s">
         <v>16</v>
       </c>
+      <c r="D151" t="s">
+        <v>24</v>
+      </c>
+      <c r="E151" t="s">
+        <v>24</v>
+      </c>
       <c r="F151">
         <v>3565.09</v>
       </c>
@@ -4184,6 +4484,12 @@
       <c r="C152" t="s">
         <v>32</v>
       </c>
+      <c r="D152" t="s">
+        <v>24</v>
+      </c>
+      <c r="E152" t="s">
+        <v>24</v>
+      </c>
       <c r="F152">
         <v>482.31</v>
       </c>
@@ -4204,6 +4510,12 @@
       <c r="C153" t="s">
         <v>34</v>
       </c>
+      <c r="D153" t="s">
+        <v>24</v>
+      </c>
+      <c r="E153" t="s">
+        <v>24</v>
+      </c>
       <c r="F153">
         <v>547.26</v>
       </c>
@@ -4224,6 +4536,12 @@
       <c r="C154" t="s">
         <v>35</v>
       </c>
+      <c r="D154" t="s">
+        <v>24</v>
+      </c>
+      <c r="E154" t="s">
+        <v>24</v>
+      </c>
       <c r="F154">
         <v>601.89</v>
       </c>
@@ -4244,6 +4562,12 @@
       <c r="C155" t="s">
         <v>36</v>
       </c>
+      <c r="D155" t="s">
+        <v>24</v>
+      </c>
+      <c r="E155" t="s">
+        <v>24</v>
+      </c>
       <c r="F155">
         <v>629.79999999999995</v>
       </c>
@@ -4264,6 +4588,12 @@
       <c r="C156" t="s">
         <v>37</v>
       </c>
+      <c r="D156" t="s">
+        <v>24</v>
+      </c>
+      <c r="E156" t="s">
+        <v>24</v>
+      </c>
       <c r="F156">
         <v>749.41</v>
       </c>
@@ -4284,6 +4614,12 @@
       <c r="C157" t="s">
         <v>38</v>
       </c>
+      <c r="D157" t="s">
+        <v>24</v>
+      </c>
+      <c r="E157" t="s">
+        <v>24</v>
+      </c>
       <c r="F157">
         <v>876.81</v>
       </c>
@@ -4304,6 +4640,12 @@
       <c r="C158" t="s">
         <v>39</v>
       </c>
+      <c r="D158" t="s">
+        <v>24</v>
+      </c>
+      <c r="E158" t="s">
+        <v>24</v>
+      </c>
       <c r="F158">
         <v>1183.72</v>
       </c>
@@ -4324,6 +4666,12 @@
       <c r="C159" t="s">
         <v>40</v>
       </c>
+      <c r="D159" t="s">
+        <v>24</v>
+      </c>
+      <c r="E159" t="s">
+        <v>24</v>
+      </c>
       <c r="F159">
         <v>1473.12</v>
       </c>
@@ -4344,6 +4692,12 @@
       <c r="C160" t="s">
         <v>41</v>
       </c>
+      <c r="D160" t="s">
+        <v>24</v>
+      </c>
+      <c r="E160" t="s">
+        <v>24</v>
+      </c>
       <c r="F160">
         <v>2062.36</v>
       </c>
@@ -4363,6 +4717,12 @@
       </c>
       <c r="C161" t="s">
         <v>16</v>
+      </c>
+      <c r="D161" t="s">
+        <v>24</v>
+      </c>
+      <c r="E161" t="s">
+        <v>24</v>
       </c>
       <c r="F161">
         <v>2893.86</v>

</xml_diff>

<commit_message>
Adicionadas faixas de preço e preferências por empresa
</commit_message>
<xml_diff>
--- a/planos_de_saude_unificado.xlsx
+++ b/planos_de_saude_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Torres\Documents\IDPB\cotacao-plano-saude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527296D8-812C-4667-9B89-C5C2230DB2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CDB468-DD58-4766-93BD-B9D12ABE89DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="36">
   <si>
     <t>Empresa</t>
   </si>
@@ -118,46 +118,13 @@
     <t>Proasa</t>
   </si>
   <si>
-    <t>00 - 18</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
     <t>2025-08</t>
-  </si>
-  <si>
-    <t>19 - 23</t>
-  </si>
-  <si>
-    <t>24 - 28</t>
-  </si>
-  <si>
-    <t>29 - 33</t>
-  </si>
-  <si>
-    <t>34 - 38</t>
-  </si>
-  <si>
-    <t>39 - 43</t>
-  </si>
-  <si>
-    <t>44 - 48</t>
-  </si>
-  <si>
-    <t>49 - 53</t>
-  </si>
-  <si>
-    <t>54 - 58</t>
   </si>
   <si>
     <t>SB Saúde</t>
   </si>
   <si>
     <t>Sem Coparticipação</t>
-  </si>
-  <si>
-    <t>00-18</t>
   </si>
   <si>
     <t>2025-07</t>
@@ -525,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="D270" sqref="D270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5392,7 +5359,7 @@
         <v>8</v>
       </c>
       <c r="C212" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D212" t="s">
         <v>13</v>
@@ -5401,10 +5368,10 @@
         <v>295.92</v>
       </c>
       <c r="F212" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G212" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -5415,7 +5382,7 @@
         <v>8</v>
       </c>
       <c r="C213" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D213" t="s">
         <v>13</v>
@@ -5424,10 +5391,10 @@
         <v>378.77</v>
       </c>
       <c r="F213" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G213" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -5438,7 +5405,7 @@
         <v>8</v>
       </c>
       <c r="C214" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D214" t="s">
         <v>13</v>
@@ -5447,10 +5414,10 @@
         <v>402.44</v>
       </c>
       <c r="F214" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G214" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -5461,7 +5428,7 @@
         <v>8</v>
       </c>
       <c r="C215" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D215" t="s">
         <v>13</v>
@@ -5470,10 +5437,10 @@
         <v>414.23</v>
       </c>
       <c r="F215" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G215" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -5484,7 +5451,7 @@
         <v>8</v>
       </c>
       <c r="C216" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D216" t="s">
         <v>13</v>
@@ -5493,10 +5460,10 @@
         <v>452.7</v>
       </c>
       <c r="F216" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G216" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -5507,7 +5474,7 @@
         <v>8</v>
       </c>
       <c r="C217" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D217" t="s">
         <v>13</v>
@@ -5516,10 +5483,10 @@
         <v>517.79999999999995</v>
       </c>
       <c r="F217" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G217" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -5530,7 +5497,7 @@
         <v>8</v>
       </c>
       <c r="C218" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D218" t="s">
         <v>13</v>
@@ -5539,10 +5506,10 @@
         <v>724.9</v>
       </c>
       <c r="F218" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G218" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -5553,7 +5520,7 @@
         <v>8</v>
       </c>
       <c r="C219" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D219" t="s">
         <v>13</v>
@@ -5562,10 +5529,10 @@
         <v>970.51</v>
       </c>
       <c r="F219" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G219" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -5576,7 +5543,7 @@
         <v>8</v>
       </c>
       <c r="C220" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D220" t="s">
         <v>13</v>
@@ -5585,10 +5552,10 @@
         <v>1088.9000000000001</v>
       </c>
       <c r="F220" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G220" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -5608,10 +5575,10 @@
         <v>1775.35</v>
       </c>
       <c r="F221" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G221" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -5622,7 +5589,7 @@
         <v>8</v>
       </c>
       <c r="C222" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D222" t="s">
         <v>13</v>
@@ -5631,10 +5598,10 @@
         <v>262.33999999999997</v>
       </c>
       <c r="F222" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G222" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -5645,7 +5612,7 @@
         <v>8</v>
       </c>
       <c r="C223" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D223" t="s">
         <v>13</v>
@@ -5654,10 +5621,10 @@
         <v>297.56</v>
       </c>
       <c r="F223" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G223" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -5668,7 +5635,7 @@
         <v>8</v>
       </c>
       <c r="C224" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D224" t="s">
         <v>13</v>
@@ -5677,10 +5644,10 @@
         <v>327.25</v>
       </c>
       <c r="F224" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G224" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -5691,7 +5658,7 @@
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D225" t="s">
         <v>13</v>
@@ -5700,10 +5667,10 @@
         <v>342.43</v>
       </c>
       <c r="F225" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G225" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -5714,7 +5681,7 @@
         <v>8</v>
       </c>
       <c r="C226" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D226" t="s">
         <v>13</v>
@@ -5723,10 +5690,10 @@
         <v>407.46</v>
       </c>
       <c r="F226" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G226" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -5737,7 +5704,7 @@
         <v>8</v>
       </c>
       <c r="C227" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D227" t="s">
         <v>13</v>
@@ -5746,10 +5713,10 @@
         <v>476.74</v>
       </c>
       <c r="F227" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G227" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -5760,7 +5727,7 @@
         <v>8</v>
       </c>
       <c r="C228" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D228" t="s">
         <v>13</v>
@@ -5769,10 +5736,10 @@
         <v>643.61</v>
       </c>
       <c r="F228" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G228" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -5783,7 +5750,7 @@
         <v>8</v>
       </c>
       <c r="C229" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D229" t="s">
         <v>13</v>
@@ -5792,10 +5759,10 @@
         <v>800.95</v>
       </c>
       <c r="F229" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G229" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -5806,7 +5773,7 @@
         <v>8</v>
       </c>
       <c r="C230" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D230" t="s">
         <v>13</v>
@@ -5815,10 +5782,10 @@
         <v>1121.3399999999999</v>
       </c>
       <c r="F230" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G230" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -5838,10 +5805,10 @@
         <v>1570.97</v>
       </c>
       <c r="F231" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G231" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -5852,7 +5819,7 @@
         <v>8</v>
       </c>
       <c r="C232" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D232" t="s">
         <v>14</v>
@@ -5861,10 +5828,10 @@
         <v>373.13</v>
       </c>
       <c r="F232" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G232" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -5875,7 +5842,7 @@
         <v>8</v>
       </c>
       <c r="C233" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D233" t="s">
         <v>14</v>
@@ -5884,10 +5851,10 @@
         <v>442.9</v>
       </c>
       <c r="F233" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G233" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -5898,7 +5865,7 @@
         <v>8</v>
       </c>
       <c r="C234" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D234" t="s">
         <v>14</v>
@@ -5907,10 +5874,10 @@
         <v>531.48</v>
       </c>
       <c r="F234" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G234" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -5921,7 +5888,7 @@
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D235" t="s">
         <v>14</v>
@@ -5930,10 +5897,10 @@
         <v>593.67999999999995</v>
       </c>
       <c r="F235" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G235" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -5944,7 +5911,7 @@
         <v>8</v>
       </c>
       <c r="C236" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D236" t="s">
         <v>14</v>
@@ -5953,10 +5920,10 @@
         <v>664.91</v>
       </c>
       <c r="F236" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G236" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -5967,7 +5934,7 @@
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D237" t="s">
         <v>14</v>
@@ -5976,10 +5943,10 @@
         <v>819.96</v>
       </c>
       <c r="F237" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G237" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -5990,7 +5957,7 @@
         <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D238" t="s">
         <v>14</v>
@@ -5999,10 +5966,10 @@
         <v>914.02</v>
       </c>
       <c r="F238" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G238" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -6013,7 +5980,7 @@
         <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D239" t="s">
         <v>14</v>
@@ -6022,10 +5989,10 @@
         <v>1269.1199999999999</v>
       </c>
       <c r="F239" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G239" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -6036,7 +6003,7 @@
         <v>8</v>
       </c>
       <c r="C240" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D240" t="s">
         <v>14</v>
@@ -6045,10 +6012,10 @@
         <v>1785.8</v>
       </c>
       <c r="F240" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G240" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -6068,10 +6035,10 @@
         <v>2234.34</v>
       </c>
       <c r="F241" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G241" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -6082,7 +6049,7 @@
         <v>8</v>
       </c>
       <c r="C242" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D242" t="s">
         <v>14</v>
@@ -6091,10 +6058,10 @@
         <v>354.17</v>
       </c>
       <c r="F242" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G242" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -6105,7 +6072,7 @@
         <v>8</v>
       </c>
       <c r="C243" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D243" t="s">
         <v>14</v>
@@ -6114,10 +6081,10 @@
         <v>401.72</v>
       </c>
       <c r="F243" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G243" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -6128,7 +6095,7 @@
         <v>8</v>
       </c>
       <c r="C244" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D244" t="s">
         <v>14</v>
@@ -6137,10 +6104,10 @@
         <v>441.8</v>
       </c>
       <c r="F244" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G244" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -6151,7 +6118,7 @@
         <v>8</v>
       </c>
       <c r="C245" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D245" t="s">
         <v>14</v>
@@ -6160,10 +6127,10 @@
         <v>462.29</v>
       </c>
       <c r="F245" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G245" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -6174,7 +6141,7 @@
         <v>8</v>
       </c>
       <c r="C246" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D246" t="s">
         <v>14</v>
@@ -6183,10 +6150,10 @@
         <v>550.1</v>
       </c>
       <c r="F246" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G246" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -6197,7 +6164,7 @@
         <v>8</v>
       </c>
       <c r="C247" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D247" t="s">
         <v>14</v>
@@ -6206,10 +6173,10 @@
         <v>643.61</v>
       </c>
       <c r="F247" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G247" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -6220,7 +6187,7 @@
         <v>8</v>
       </c>
       <c r="C248" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D248" t="s">
         <v>14</v>
@@ -6229,10 +6196,10 @@
         <v>868.89</v>
       </c>
       <c r="F248" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G248" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -6243,7 +6210,7 @@
         <v>8</v>
       </c>
       <c r="C249" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D249" t="s">
         <v>14</v>
@@ -6252,10 +6219,10 @@
         <v>1081.32</v>
       </c>
       <c r="F249" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G249" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -6266,7 +6233,7 @@
         <v>8</v>
       </c>
       <c r="C250" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D250" t="s">
         <v>14</v>
@@ -6275,10 +6242,10 @@
         <v>1513.85</v>
       </c>
       <c r="F250" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G250" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -6298,10 +6265,10 @@
         <v>2120.81</v>
       </c>
       <c r="F251" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G251" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -6312,7 +6279,7 @@
         <v>8</v>
       </c>
       <c r="C252" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D252" t="s">
         <v>14</v>
@@ -6321,10 +6288,10 @@
         <v>594.27</v>
       </c>
       <c r="F252" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G252" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -6335,7 +6302,7 @@
         <v>8</v>
       </c>
       <c r="C253" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D253" t="s">
         <v>14</v>
@@ -6344,10 +6311,10 @@
         <v>760.63</v>
       </c>
       <c r="F253" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G253" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -6358,7 +6325,7 @@
         <v>8</v>
       </c>
       <c r="C254" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D254" t="s">
         <v>14</v>
@@ -6367,10 +6334,10 @@
         <v>808.05</v>
       </c>
       <c r="F254" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G254" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -6381,7 +6348,7 @@
         <v>8</v>
       </c>
       <c r="C255" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D255" t="s">
         <v>14</v>
@@ -6390,10 +6357,10 @@
         <v>831.82</v>
       </c>
       <c r="F255" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G255" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -6404,7 +6371,7 @@
         <v>8</v>
       </c>
       <c r="C256" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D256" t="s">
         <v>14</v>
@@ -6413,10 +6380,10 @@
         <v>909.05</v>
       </c>
       <c r="F256" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G256" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -6427,7 +6394,7 @@
         <v>8</v>
       </c>
       <c r="C257" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D257" t="s">
         <v>14</v>
@@ -6436,10 +6403,10 @@
         <v>1039.76</v>
       </c>
       <c r="F257" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G257" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -6450,7 +6417,7 @@
         <v>8</v>
       </c>
       <c r="C258" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D258" t="s">
         <v>14</v>
@@ -6459,10 +6426,10 @@
         <v>1455.73</v>
       </c>
       <c r="F258" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G258" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -6473,7 +6440,7 @@
         <v>8</v>
       </c>
       <c r="C259" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D259" t="s">
         <v>14</v>
@@ -6482,10 +6449,10 @@
         <v>1948.96</v>
       </c>
       <c r="F259" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G259" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -6496,7 +6463,7 @@
         <v>8</v>
       </c>
       <c r="C260" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D260" t="s">
         <v>14</v>
@@ -6505,10 +6472,10 @@
         <v>2186.75</v>
       </c>
       <c r="F260" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G260" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -6528,10 +6495,10 @@
         <v>3565.09</v>
       </c>
       <c r="F261" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G261" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -6542,7 +6509,7 @@
         <v>8</v>
       </c>
       <c r="C262" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D262" t="s">
         <v>14</v>
@@ -6551,10 +6518,10 @@
         <v>482.31</v>
       </c>
       <c r="F262" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G262" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -6565,7 +6532,7 @@
         <v>8</v>
       </c>
       <c r="C263" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D263" t="s">
         <v>14</v>
@@ -6574,10 +6541,10 @@
         <v>547.26</v>
       </c>
       <c r="F263" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G263" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -6588,7 +6555,7 @@
         <v>8</v>
       </c>
       <c r="C264" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D264" t="s">
         <v>14</v>
@@ -6597,10 +6564,10 @@
         <v>601.89</v>
       </c>
       <c r="F264" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G264" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -6611,7 +6578,7 @@
         <v>8</v>
       </c>
       <c r="C265" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D265" t="s">
         <v>14</v>
@@ -6620,10 +6587,10 @@
         <v>629.79999999999995</v>
       </c>
       <c r="F265" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G265" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
@@ -6634,7 +6601,7 @@
         <v>8</v>
       </c>
       <c r="C266" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D266" t="s">
         <v>14</v>
@@ -6643,10 +6610,10 @@
         <v>749.41</v>
       </c>
       <c r="F266" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G266" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
@@ -6657,7 +6624,7 @@
         <v>8</v>
       </c>
       <c r="C267" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D267" t="s">
         <v>14</v>
@@ -6666,10 +6633,10 @@
         <v>876.81</v>
       </c>
       <c r="F267" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G267" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
@@ -6680,7 +6647,7 @@
         <v>8</v>
       </c>
       <c r="C268" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D268" t="s">
         <v>14</v>
@@ -6689,10 +6656,10 @@
         <v>1183.72</v>
       </c>
       <c r="F268" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G268" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
@@ -6703,7 +6670,7 @@
         <v>8</v>
       </c>
       <c r="C269" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D269" t="s">
         <v>14</v>
@@ -6712,10 +6679,10 @@
         <v>1473.12</v>
       </c>
       <c r="F269" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G269" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -6726,7 +6693,7 @@
         <v>8</v>
       </c>
       <c r="C270" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D270" t="s">
         <v>14</v>
@@ -6735,10 +6702,10 @@
         <v>2062.36</v>
       </c>
       <c r="F270" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G270" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
@@ -6758,21 +6725,21 @@
         <v>2893.86</v>
       </c>
       <c r="F271" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G271" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B272" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C272" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D272" t="s">
         <v>13</v>
@@ -6781,7 +6748,7 @@
         <v>174.49</v>
       </c>
       <c r="F272" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G272" t="s">
         <v>10</v>
@@ -6789,13 +6756,13 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B273" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C273" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D273" t="s">
         <v>14</v>
@@ -6804,7 +6771,7 @@
         <v>255.42</v>
       </c>
       <c r="F273" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G273" t="s">
         <v>10</v>
@@ -6812,10 +6779,10 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B274" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C274" t="s">
         <v>15</v>
@@ -6827,7 +6794,7 @@
         <v>225.69</v>
       </c>
       <c r="F274" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G274" t="s">
         <v>10</v>
@@ -6835,10 +6802,10 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B275" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C275" t="s">
         <v>15</v>
@@ -6850,7 +6817,7 @@
         <v>369.98</v>
       </c>
       <c r="F275" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G275" t="s">
         <v>10</v>
@@ -6858,10 +6825,10 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B276" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C276" t="s">
         <v>16</v>
@@ -6873,7 +6840,7 @@
         <v>252.76</v>
       </c>
       <c r="F276" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G276" t="s">
         <v>10</v>
@@ -6881,10 +6848,10 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B277" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C277" t="s">
         <v>16</v>
@@ -6896,7 +6863,7 @@
         <v>406.58</v>
       </c>
       <c r="F277" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G277" t="s">
         <v>10</v>
@@ -6904,10 +6871,10 @@
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B278" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C278" t="s">
         <v>17</v>
@@ -6919,7 +6886,7 @@
         <v>283.08</v>
       </c>
       <c r="F278" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G278" t="s">
         <v>10</v>
@@ -6927,10 +6894,10 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B279" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C279" t="s">
         <v>17</v>
@@ -6942,7 +6909,7 @@
         <v>414.43</v>
       </c>
       <c r="F279" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G279" t="s">
         <v>10</v>
@@ -6950,10 +6917,10 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B280" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C280" t="s">
         <v>18</v>
@@ -6965,7 +6932,7 @@
         <v>318.67</v>
       </c>
       <c r="F280" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G280" t="s">
         <v>10</v>
@@ -6973,10 +6940,10 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B281" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C281" t="s">
         <v>18</v>
@@ -6988,7 +6955,7 @@
         <v>466.5</v>
       </c>
       <c r="F281" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G281" t="s">
         <v>10</v>
@@ -6996,10 +6963,10 @@
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B282" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C282" t="s">
         <v>19</v>
@@ -7011,7 +6978,7 @@
         <v>359.24</v>
       </c>
       <c r="F282" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G282" t="s">
         <v>10</v>
@@ -7019,10 +6986,10 @@
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B283" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C283" t="s">
         <v>19</v>
@@ -7034,7 +7001,7 @@
         <v>525.9</v>
       </c>
       <c r="F283" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G283" t="s">
         <v>10</v>
@@ -7042,10 +7009,10 @@
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B284" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C284" t="s">
         <v>20</v>
@@ -7057,7 +7024,7 @@
         <v>449.07</v>
       </c>
       <c r="F284" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G284" t="s">
         <v>10</v>
@@ -7065,10 +7032,10 @@
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B285" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C285" t="s">
         <v>20</v>
@@ -7080,7 +7047,7 @@
         <v>657.38</v>
       </c>
       <c r="F285" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G285" t="s">
         <v>10</v>
@@ -7088,10 +7055,10 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B286" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C286" t="s">
         <v>21</v>
@@ -7103,7 +7070,7 @@
         <v>538.88</v>
       </c>
       <c r="F286" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G286" t="s">
         <v>10</v>
@@ -7111,10 +7078,10 @@
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B287" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C287" t="s">
         <v>21</v>
@@ -7126,7 +7093,7 @@
         <v>788.85</v>
       </c>
       <c r="F287" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G287" t="s">
         <v>10</v>
@@ -7134,10 +7101,10 @@
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B288" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C288" t="s">
         <v>22</v>
@@ -7149,7 +7116,7 @@
         <v>733.84</v>
       </c>
       <c r="F288" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G288" t="s">
         <v>10</v>
@@ -7157,10 +7124,10 @@
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B289" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C289" t="s">
         <v>22</v>
@@ -7172,7 +7139,7 @@
         <v>1074.25</v>
       </c>
       <c r="F289" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G289" t="s">
         <v>10</v>
@@ -7180,10 +7147,10 @@
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B290" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C290" t="s">
         <v>23</v>
@@ -7195,7 +7162,7 @@
         <v>1039.8900000000001</v>
       </c>
       <c r="F290" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G290" t="s">
         <v>10</v>
@@ -7203,10 +7170,10 @@
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B291" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C291" t="s">
         <v>23</v>
@@ -7218,7 +7185,7 @@
         <v>1522.23</v>
       </c>
       <c r="F291" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G291" t="s">
         <v>10</v>

</xml_diff>